<commit_message>
changed to new repo
</commit_message>
<xml_diff>
--- a/project1devs/disagreements.xlsx
+++ b/project1devs/disagreements.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,38 +488,38 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Carlos Cañizares Estévez</t>
+          <t>0x0is1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>c.canizaresestevez@hotmail.com</t>
+          <t>0x0is1@protonmail.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Carlos Cañizares Estévez</t>
+          <t>Not Your Surya</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ccanizares@plainconcepts.com</t>
+          <t>0x0is1@protonmail.com</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -530,22 +530,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Christian Arenas</t>
+          <t>APILayer</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>carenas@plainconcepts.com</t>
+          <t>75280960+apilayer-admin@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Christian Arenas</t>
+          <t>apilayer</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>christian.arenasnavarro@hotmail.com</t>
+          <t>support@apilayer.net</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -558,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -572,38 +572,38 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Christian Arenas</t>
+          <t>APILayer</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>carenas@plainconcepts.com</t>
+          <t>75280960+apilayer-admin@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Christian Arenas</t>
+          <t>apilayer-admin</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>christian147_@hotmail.com</t>
+          <t>75280960+apilayer-admin@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -614,22 +614,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Daniyar Alpyspayev</t>
+          <t>AadityaMunjal</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>daniyar.alpyspayev@gmail.com</t>
+          <t>69916707+AadityaMunjal@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Daniyar Alpyspayev</t>
+          <t>AadityaMunjal</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>daniyara@thereachagency.com</t>
+          <t>aadityamunjal06@gmail.com</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -642,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -656,26 +656,26 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>David Sanz</t>
+          <t>Alaric Hadef</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>dsanz@plainconcepts.com</t>
+          <t>alaric.hadef@weezevent.com</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>David Sanz</t>
+          <t>alarichadef</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>dsrodenas@users.noreply.github.com</t>
+          <t>alarichadef@gmail.com</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -684,40 +684,40 @@
         <v>0</v>
       </c>
       <c r="H6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FP</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Igor Sychev</t>
+          <t>Alejandro Mesa</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>igorsych@Microsoft.com</t>
+          <t>alejandro.suarez@jam3.com</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Igor Sychev</t>
+          <t>Alejandro Mesa Suarez</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>sychev-igor.90@mail.ru</t>
+          <t>alejandro.mesa1991@gmail.com</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -729,7 +729,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -740,22 +740,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Igor Sychev</t>
+          <t>Andrea López Suárez</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>igorsych@microsoft.com</t>
+          <t>60515012+andrealps@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Igor Sychev</t>
+          <t>Andrea López Suárez</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>sychev-igor.90@mail.ru</t>
+          <t>uo264703@uniovi.es</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -768,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -782,32 +782,32 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IgorSychev</t>
+          <t>Anghel Valentin</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>igorsychev@microsoft.com</t>
+          <t>valentin_anghel_2005@hotmail.com</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Igor_Sychev</t>
+          <t>anghelvalentin</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Igor@Sychev.com</t>
+          <t>valentin_anghel_2005@hotmail.com</t>
         </is>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -824,38 +824,38 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ivan Buha</t>
+          <t>Ankur H. Singh</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ivan.Buha@communitybrands.com</t>
+          <t>49074231+sankur-codes@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Ivan Buha</t>
+          <t>sankur-codes</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ivanbuha@outlook.com</t>
+          <t>49074231+sankur-codes@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -866,29 +866,29 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Javier Suárez Ruiz</t>
+          <t>Anton</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>javiersuarezruiz@hotmail.com</t>
+          <t>anton@troppmann.xyz</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Javier Suárez Ruiz</t>
+          <t>Anton Strömkvist</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>jsuarez@plainconcepts.com</t>
+          <t>anton@stromkvist.com</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="b">
         <v>0</v>
@@ -897,7 +897,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -908,38 +908,38 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Javier Suárez Ruiz</t>
+          <t>Augustas</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>javiersuarezruiz@hotmail.com</t>
+          <t>reg1nt1z@gmail.com</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Javier Suárez Ruiz</t>
+          <t>AugustasV</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>jsuarez@plainconcepts.com</t>
+          <t>reg1nt1z@gmail.com</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
       </c>
       <c r="I12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -950,22 +950,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Kyle White</t>
+          <t>Ayush Mishra</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>kyle@xamarin.com</t>
+          <t>47855161+Beyonday008@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Kyle White</t>
+          <t>Ayush Mishra</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>kywhi@microsoft.com</t>
+          <t>ayushmishra063@gmail.com</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -978,7 +978,7 @@
         <v>0</v>
       </c>
       <c r="H13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
@@ -992,22 +992,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Lee Dumond</t>
+          <t>Benjamin Taylor</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Lee_Dumond@aisreview.com</t>
+          <t>0xBenjamin@protonmail.com</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Lee Dumond</t>
+          <t>Benjamin Taylor</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>leedumond@gmail.com</t>
+          <t>49266701+0xBenjaminTaylor@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -1020,7 +1020,7 @@
         <v>0</v>
       </c>
       <c r="H14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
@@ -1034,29 +1034,29 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Marcos Cobeña Morián</t>
+          <t>Bert</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>mcobena@plainconcepts.com</t>
+          <t>bert.marcelis@outlook.com</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Marcos Cobeña Morián</t>
+          <t>Bert Marcelis</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>marcoscm.digital@gmail.com</t>
+          <t>bert.marcelis@samtrafiken.se</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -1065,7 +1065,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1076,38 +1076,38 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Mateusz Karkula</t>
+          <t>Boxfort</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>karql.pl@gmail.com</t>
+          <t>jackwanderson@protonmail.com</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Mateusz Karkula</t>
+          <t>Jack Anderson</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>mateusz.karkula@comarch.com</t>
+          <t>jackwanderson@protonmail.com</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
       </c>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1118,38 +1118,38 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Miguel Veloso</t>
+          <t>Bradley Juma</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>mveloso@plainconcepts.com</t>
+          <t>bradleyjuma170@gmail.com</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Miguel Veloso</t>
+          <t>bradley-Amuj</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>mvelosop@gmail.com</t>
+          <t>bradleyjuma170@gmail.com</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="F17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="b">
         <v>0</v>
       </c>
       <c r="I17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1160,38 +1160,38 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Nish</t>
+          <t>Chanwit Piromplad</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>nish@xamarin.com</t>
+          <t>kingkong2103@gmail.com</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Nish</t>
+          <t>tonpc64</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>nnish@live.com</t>
+          <t>kingkong2103@gmail.com</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
       </c>
       <c r="I18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1202,22 +1202,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Nish Anil</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>nanil@microsoft.com</t>
+          <t>danielarezdiaz@gmail.com</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Nish Anil</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>nish@xamarin.com</t>
+          <t>danzanzu@gmail.com</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -1227,7 +1227,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -1237,45 +1237,45 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TP</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Nish Anil</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>nanil@microsoft.com</t>
+          <t>danielarezdiaz@gmail.com</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Nish Anil</t>
+          <t>Mister Rajoy</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>nnish@live.com</t>
+          <t>danielarezdiaz@gmail.com</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
       </c>
       <c r="I20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1286,22 +1286,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Nish Anil</t>
+          <t>Dave Machado</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>nish@microsoft.com</t>
+          <t>dave@davemachado.com</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Nish Anil</t>
+          <t>Dave Machado</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>nnish@live.com</t>
+          <t>davemachado@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1314,7 +1314,7 @@
         <v>0</v>
       </c>
       <c r="H21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
@@ -1328,38 +1328,38 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Nish Anil</t>
+          <t>Dave Machado</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>nish@xamarin.com</t>
+          <t>dave@davemachado.com</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Nish Anil</t>
+          <t>davemachado</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>nnish@live.com</t>
+          <t>dave@davemachado.com</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
       </c>
       <c r="I22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1370,26 +1370,26 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Ramón Tomás</t>
+          <t>Dave Machado</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ramon.tomas84@hotmail.com</t>
+          <t>davemachado@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Ramón Tomás</t>
+          <t>davemachado</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>rtomas@plainconcepts.com</t>
+          <t>dave@davemachado.com</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -1398,10 +1398,10 @@
         <v>0</v>
       </c>
       <c r="H23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1412,38 +1412,38 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Reuben Bond</t>
+          <t>David</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>rebond@microsoft.com</t>
+          <t>62877244+ThatCopy@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Reuben Bond</t>
+          <t>ThatCopy</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>reuben.bond@gmail.com</t>
+          <t>62877244+ThatCopy@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1454,26 +1454,26 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Unai Zorrilla Castro</t>
+          <t>David Davó</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Unai Zorrilla Castro</t>
+          <t>david@ddavo.me</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Unai Zorrilla Castro</t>
+          <t>DavidsDvm</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>unai@plainconcepts.com</t>
+          <t>33884578+DavidsDvm@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -1482,10 +1482,10 @@
         <v>0</v>
       </c>
       <c r="H25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1496,29 +1496,29 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Rafsanul Hasan</t>
+          <t>David Katz</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>rafsanulhasan@outlook.com</t>
+          <t>15Dkatz@shcp.edu</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>rafsanulhasan</t>
+          <t>David Katz</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>rafsanulhasan@RHPC-MSI</t>
+          <t>dkatz@zendesk.com</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" t="b">
         <v>0</v>
@@ -1527,7 +1527,7 @@
         <v>0</v>
       </c>
       <c r="I26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1538,32 +1538,32 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Bill Wagner</t>
+          <t>Dylan Delobel</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>wiwagn@microsoft.com</t>
+          <t>dylan.delobel66@gmail.com</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>BillWagner</t>
+          <t>DylanDelobel</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>bill.w.wagner@outlook.com</t>
+          <t>dylan.delobel66@gmail.com</t>
         </is>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" t="b">
         <v>0</v>
@@ -1580,38 +1580,38 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Igor Sychev</t>
+          <t>Eric Wyne</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>igorsych@Microsoft.com</t>
+          <t>ecwyne@gmail.com</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>IgorSychev</t>
+          <t>Eric Wyne</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>igorsychev@microsoft.com</t>
+          <t>ecwyne@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1622,38 +1622,38 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Igor Sychev</t>
+          <t>Farhan Salam</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>igorsych@Microsoft.com</t>
+          <t>faaann@gmail.com</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Igor_Sychev</t>
+          <t>farhansalam</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Igor@Sychev.com</t>
+          <t>faaann@gmail.com</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" t="b">
         <v>0</v>
       </c>
       <c r="I29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -1664,38 +1664,38 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Igor Sychev</t>
+          <t>Fayas Noushad</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>igorsych@microsoft.com</t>
+          <t>76828314+FayasNoushad@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>IgorSychev</t>
+          <t>Fayas Noushad</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>igorsychev@microsoft.com</t>
+          <t>TheFayasNoushad@gmail.com</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
       </c>
       <c r="G30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -1706,32 +1706,32 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Igor Sychev</t>
+          <t>Filip Molčík</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>igorsych@microsoft.com</t>
+          <t>fmolda@seznam.cz</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Igor_Sychev</t>
+          <t>molcik</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Igor@Sychev.com</t>
+          <t>fmolda@seznam.cz</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" t="b">
         <v>0</v>
@@ -1748,38 +1748,38 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Igor Sychev</t>
+          <t>Filip Molčík</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>sychev-igor.90@mail.ru</t>
+          <t>fmolda@seznam.cz</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>IgorSychev</t>
+          <t>molcik</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>igorsychev@microsoft.com</t>
+          <t>fmolda@seznam.cz</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" t="b">
         <v>0</v>
       </c>
       <c r="I32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -1790,22 +1790,22 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Igor Sychev</t>
+          <t>Gunter Thomas</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>sychev-igor.90@mail.ru</t>
+          <t>github@gunterthomas.com</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Igor_Sychev</t>
+          <t>Gunter Thomas</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Igor@Sychev.com</t>
+          <t>gunter.thomas@check24.de</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1832,26 +1832,26 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Sychev Igor</t>
+          <t>Gunter Thomas</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>igorsych@microsoft.com</t>
+          <t>gunter.thomas@check24.de</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>SychevIgor</t>
+          <t>Gunter Thomas</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>SychevIgor@users.noreply.github.com</t>
+          <t>gunter@gunterthomas.com</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
@@ -1860,10 +1860,10 @@
         <v>0</v>
       </c>
       <c r="H34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -1874,32 +1874,32 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Erik Pique</t>
+          <t>Guy Edwards</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>epique@plainconcepts.com</t>
+          <t>guyfedwards@gmail.com</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>erikpique</t>
+          <t>guyfedwards</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>erik.pique@gmail.com</t>
+          <t>guyfedwards@gmail.com</t>
         </is>
       </c>
       <c r="E35" t="n">
         <v>0</v>
       </c>
       <c r="F35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
@@ -1916,22 +1916,22 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CESARDELATORRE</t>
+          <t>Gyeongjun Paik</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CESARDL@MICROSOFT.COM</t>
+          <t>paikend@gmail.com</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Cesar De la Torre</t>
+          <t>paikend</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>cesardl@Cesars-MacBook-Pro.local</t>
+          <t>paikend@gmail.com</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1941,10 +1941,10 @@
         <v>1</v>
       </c>
       <c r="G36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
@@ -1958,38 +1958,38 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CESARDELATORRE</t>
+          <t>Hakan Ensari</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>CESARDL@MICROSOFT.COM</t>
+          <t>hakanensari@gmail.com</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Cesar De la Torre</t>
+          <t>Hakan Ensari</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>cesardl@microsoft.com</t>
+          <t>hakanensari@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" t="b">
         <v>1</v>
       </c>
       <c r="G37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -2000,29 +2000,29 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CESARDELATORRE</t>
+          <t>Hamid Reza Mohammadi</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>cesardl@microsoft.com</t>
+          <t>hrmoh@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Cesar De la Torre</t>
+          <t>Hamid Reza Mohammadi</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>cesardl@Cesars-MacBook-Pro.local</t>
+          <t>mohammadi.hr@gmail.com</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" t="b">
         <v>0</v>
@@ -2031,7 +2031,7 @@
         <v>1</v>
       </c>
       <c r="I38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -2042,38 +2042,38 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>CESARDELATORRE</t>
+          <t>Harish Kotra</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>cesardl@microsoft.com</t>
+          <t>harishkotra@gmail.com</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Cesar De la Torre</t>
+          <t>Harish Kotra</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>cesardl@microsoft.com</t>
+          <t>harishkotra@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" t="b">
         <v>1</v>
       </c>
       <c r="G39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -2084,29 +2084,29 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>IgorSychev</t>
+          <t>Heitor Gouvea</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>igorsychev@microsoft.com</t>
+          <t>hi@heitorgouvea.me</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>igorsych</t>
+          <t>HeitorG</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>igorsych@microsoft.com</t>
+          <t>hi@heitorgouvea.me</t>
         </is>
       </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
       <c r="F40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" t="b">
         <v>1</v>
@@ -2126,35 +2126,35 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Igor_Sychev</t>
+          <t>Himanshu Sharma</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Igor@Sychev.com</t>
+          <t>88159798+sh-himanshu@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>igorsych</t>
+          <t>sh-himanshu</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>igorsych@microsoft.com</t>
+          <t>88159798+sh-himanshu@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="F41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" t="b">
         <v>0</v>
@@ -2168,22 +2168,22 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Igor Sychev</t>
+          <t>IP Location</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>igorsych@Microsoft.com</t>
+          <t>hello@ipapi.co</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>igorsych</t>
+          <t>ipapi-co</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>igorsych@microsoft.com</t>
+          <t>hello@ipapi.co</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -2210,38 +2210,38 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Igor Sychev</t>
+          <t>Ian Havelock</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>igorsych@microsoft.com</t>
+          <t>Morrolan@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>igorsych</t>
+          <t>Ian Havelock</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>igorsych@microsoft.com</t>
+          <t>ian@morrolan.com</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -2252,29 +2252,29 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Igor Sychev</t>
+          <t>James Brooks</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>sychev-igor.90@mail.ru</t>
+          <t>james@alt-three.com</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>igorsych</t>
+          <t>James Brooks</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>igorsych@microsoft.com</t>
+          <t>james@bluebaytravel.co.uk</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" t="b">
         <v>0</v>
@@ -2283,7 +2283,7 @@
         <v>0</v>
       </c>
       <c r="I44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -2294,26 +2294,26 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Stepan</t>
+          <t>James Brooks</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>kologicdev@icloud.com</t>
+          <t>james@alt-three.com</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>n-stefan</t>
+          <t>James Brooks</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>38526229+n-stefan@users.noreply.github.com</t>
+          <t>jbrooksuk@me.com</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
@@ -2322,10 +2322,10 @@
         <v>0</v>
       </c>
       <c r="H45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -2336,26 +2336,26 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Gajendra Babu Thokala [MSFT]</t>
+          <t>James Brooks</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>gajendra.babu@hotmail.com</t>
+          <t>james@bluebaytravel.co.uk</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Gajendra Thokala</t>
+          <t>James Brooks</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>gababu@microsoft.com</t>
+          <t>jbrooksuk@me.com</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F46" t="b">
         <v>0</v>
@@ -2367,7 +2367,7 @@
         <v>0</v>
       </c>
       <c r="I46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -2378,26 +2378,26 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Unai Zorrilla Castro</t>
+          <t>James Wright</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Unai Zorrilla Castro</t>
+          <t>james.wright@net-a-porter.com</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>unaizorrilla</t>
+          <t>James Wright</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>unai@plainconcepts.com</t>
+          <t>james@jamesswright.co.uk</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" t="b">
         <v>0</v>
@@ -2409,7 +2409,7 @@
         <v>0</v>
       </c>
       <c r="I47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -2420,32 +2420,32 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Unai Zorrilla Castro</t>
+          <t>Joaquin Montesinos</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>unai@plainconcepts.com</t>
+          <t>jkm280294@gmail.com</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>unaizorrilla</t>
+          <t>Joaquin Montesinos Muñoz</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>unai@plainconcepts.com</t>
+          <t>ge72def@tum.de</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H48" t="b">
         <v>0</v>
@@ -2462,26 +2462,26 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Borja García</t>
+          <t>Johan Naizu</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>borjasanes@hotmail.com</t>
+          <t>68628917+johan-naizu@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Borja García Rodríguez</t>
+          <t>Johan Naizu</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>bgarcia@plainconcepts.com</t>
+          <t>johan@naizu.in</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0.6666666666666666</v>
+        <v>1</v>
       </c>
       <c r="F49" t="b">
         <v>0</v>
@@ -2490,10 +2490,10 @@
         <v>0</v>
       </c>
       <c r="H49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -2504,38 +2504,38 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>CESARDELATORRE</t>
+          <t>Josiah Sayers</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>CESARDL@MICROSOFT.COM</t>
+          <t>47199245+JosiahSayers@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Cesar De la Torre Llorente</t>
+          <t>Josiah Sayers</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>cesardl@microsoft.com</t>
+          <t>josiah.sayers15@gmail.com</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -2546,38 +2546,38 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>CESARDELATORRE</t>
+          <t>Julien CROUZET</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>cesardl@microsoft.com</t>
+          <t>contact@juliencrouzet.fr</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Cesar De la Torre Llorente</t>
+          <t>Julien CROUZET</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>cesardl@microsoft.com</t>
+          <t>jcrouzet.actemaconsulting@tf1.fr</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51" t="b">
         <v>0</v>
       </c>
       <c r="I51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -2588,29 +2588,29 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>CESARDELATORRE</t>
+          <t>Julien Salinas</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>CESARDL@MICROSOFT.COM</t>
+          <t>all@juliensalinas.com</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>CESARDL</t>
+          <t>Julien Salinas</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>CESARDL@SURFBOOKCESARDL</t>
+          <t>julien.enilrahc@gmail.com</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52" t="b">
         <v>0</v>
@@ -2619,7 +2619,7 @@
         <v>0</v>
       </c>
       <c r="I52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -2630,26 +2630,26 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>David Sanz</t>
+          <t>Karl Hughes</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>dsanz@plainconcepts.com</t>
+          <t>khughes.me@gmail.com</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>dsanz</t>
+          <t>Karl L. Hughes</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>dsanz@plainconcepts.com</t>
+          <t>khughes.me@gmail.com</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F53" t="b">
         <v>1</v>
@@ -2661,7 +2661,7 @@
         <v>0</v>
       </c>
       <c r="I53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -2672,38 +2672,38 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Eduard Tomas</t>
+          <t>Kristian Kramer</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>etomas@gmail.com</t>
+          <t>hello@kk.dev</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>etomas</t>
+          <t>Kristian Kramer</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>etomas@gmail.com</t>
+          <t>kristian@beyondcoin.io</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54" t="b">
         <v>0</v>
       </c>
       <c r="I54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -2714,38 +2714,38 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Eduard Tomàs</t>
+          <t>KwongTN</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>etomas@gmail.com</t>
+          <t>5886584+kwongtn@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>etomas</t>
+          <t>KwongTN</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>etomas@gmail.com</t>
+          <t>tungnan5636@gmail.com</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -2756,35 +2756,35 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>José Corral</t>
+          <t>Kyle Calica</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>jcorral@plainconcepts.com</t>
+          <t>stcalica@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>jmanuelcorral</t>
+          <t>stcalica</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>jcorral@plainconcepts.com</t>
+          <t>kycalica@gmail.com</t>
         </is>
       </c>
       <c r="E56" t="n">
         <v>0</v>
       </c>
       <c r="F56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" t="b">
         <v>0</v>
@@ -2798,38 +2798,38 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>RamonTC</t>
+          <t>Leah Tabush</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>ramon.tomas84@hotmail.com</t>
+          <t>73200321+leahfern@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Ramón Tomás</t>
+          <t>Leah Tabush</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>ramon.tomas84@hotmail.com</t>
+          <t>leahtabush@gmail.com</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -2840,26 +2840,26 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>RamonTC</t>
+          <t>Lukas Panni</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>ramon.tomas84@hotmail.com</t>
+          <t>lukas-panni@web.de</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Ramón Tomás</t>
+          <t>Lukas Panni</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>rtomas@plainconcepts.com</t>
+          <t>lukas.panni@outlook.de</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58" t="b">
         <v>0</v>
@@ -2871,7 +2871,7 @@
         <v>0</v>
       </c>
       <c r="I58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -2882,38 +2882,38 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Eric Erhardt</t>
+          <t>MC Naveen</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>eric.erhardt@microsoft.com</t>
+          <t>funmemcn@gmail.com</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Eric Torre</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>etorreg@gmail.com</t>
+          <t>mailtomassnaveen@gmail.com</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="F59" t="b">
         <v>0</v>
       </c>
       <c r="G59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59" t="b">
         <v>0</v>
       </c>
       <c r="I59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -2924,38 +2924,38 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Glenn Condron</t>
+          <t>Marco Biedermann</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>glennc@microsoft.com</t>
+          <t>hello@marcobiedermann.com</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>glennc</t>
+          <t>Marco Biedermann</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>glennc@microsoft.com</t>
+          <t>marco.biedermann@gmx.de</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60" t="b">
         <v>0</v>
       </c>
       <c r="I60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -2966,26 +2966,26 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Ivan</t>
+          <t>Marek Dano</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>ivanbuha@outlook.com</t>
+          <t>marekdano@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Ivan Buha</t>
+          <t>Marek Dano</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Ivan.Buha@communitybrands.com</t>
+          <t>mk.dano@gmail.com</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F61" t="b">
         <v>0</v>
@@ -2994,10 +2994,10 @@
         <v>0</v>
       </c>
       <c r="H61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -3008,38 +3008,38 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Ivan</t>
+          <t>Marios Georgiou</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>ivanbuha@outlook.com</t>
+          <t>mariosge90@gmail.com</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Ivan Buha</t>
+          <t>Marios Georgiou</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>ivanbuha@outlook.com</t>
+          <t>mgeorgiou@Ginas-MacBook-Air.local</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -3050,38 +3050,38 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Nish</t>
+          <t>Matheus Felipe</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>nish@xamarin.com</t>
+          <t>50463866+matheusfelipeog@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Nish Anil</t>
+          <t>Matheus Felipe</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>nish@microsoft.com</t>
+          <t>matheusfelipeog@protonmail.com</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G63" t="b">
         <v>0</v>
       </c>
       <c r="H63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -3092,35 +3092,35 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Nish</t>
+          <t>Mauricio Giraldo</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>nish@xamarin.com</t>
+          <t>mgiraldo@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Nish Anil</t>
+          <t>Mauricio Robayo</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>nish@xamarin.com</t>
+          <t>rfmajo@gmail.com</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>0.5</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="F64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I64" t="b">
         <v>0</v>
@@ -3134,32 +3134,32 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Nish</t>
+          <t>Maxime Nory</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>nish@xamarin.com</t>
+          <t>mxmnry@gmail.com</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Nish Anil</t>
+          <t>maxime-mn</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>nnish@live.com</t>
+          <t>maxime.mion@gmail.com</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>0.5</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="F65" t="b">
         <v>0</v>
       </c>
       <c r="G65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65" t="b">
         <v>0</v>
@@ -3176,26 +3176,26 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Nish</t>
+          <t>Michael Lynch</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>nnish@live.com</t>
+          <t>git@mtlynch.io</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Nish Anil</t>
+          <t>Michael Lynch</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>nish@microsoft.com</t>
+          <t>mtlynch@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F66" t="b">
         <v>0</v>
@@ -3204,10 +3204,10 @@
         <v>0</v>
       </c>
       <c r="H66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -3218,26 +3218,26 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Nish</t>
+          <t>Mike Street</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>nnish@live.com</t>
+          <t>mike@liquidlight.co.uk</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Nish Anil</t>
+          <t>Mike Street</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>nish@xamarin.com</t>
+          <t>mikestreety@gmail.com</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F67" t="b">
         <v>0</v>
@@ -3249,7 +3249,7 @@
         <v>0</v>
       </c>
       <c r="I67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -3260,26 +3260,26 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Nish</t>
+          <t>Milos Stojanovic</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>nnish@live.com</t>
+          <t>alcalbg@gmail.com</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Nish Anil</t>
+          <t>alcalbg</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>nnish@live.com</t>
+          <t>alcalbg@gmail.com</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F68" t="b">
         <v>1</v>
@@ -3302,29 +3302,29 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>IgorSychev</t>
+          <t>Mohamed Sohail</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>igorsychev@microsoft.com</t>
+          <t>sohailsameja@gmail.com</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Sychev Igor</t>
+          <t>Mohammed Sohail</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>igorsych@microsoft.com</t>
+          <t>sohailsameja@gmail.com</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="F69" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G69" t="b">
         <v>1</v>
@@ -3333,7 +3333,7 @@
         <v>0</v>
       </c>
       <c r="I69" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -3344,32 +3344,32 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Igor Sychev</t>
+          <t>Mori</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>sychev-igor.90@mail.ru</t>
+          <t>moriakaice@gmail.com</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Sychev Igor</t>
+          <t>moriakaice</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>igorsych@microsoft.com</t>
+          <t>moriakaice@gmail.com</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F70" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G70" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H70" t="b">
         <v>0</v>
@@ -3386,26 +3386,26 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Jose</t>
+          <t>Nirjas Jakilim</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>jose.manuel.corral@gmail.com</t>
+          <t>Nirzak@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>José Corral</t>
+          <t>Nirjas Jakilim</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>jcorral@plainconcepts.com</t>
+          <t>nirjas01@student.sust.edu</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F71" t="b">
         <v>0</v>
@@ -3414,10 +3414,10 @@
         <v>0</v>
       </c>
       <c r="H71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -3428,26 +3428,26 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Juan Antonio Cano</t>
+          <t>Pawel Borkar</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>jacanosalado@gmail.com</t>
+          <t>36134699+PawelBorkar@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>jacano</t>
+          <t>Pawel Borkar</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>jacanosalado@gmail.com</t>
+          <t>36134699+pawelborkar@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F72" t="b">
         <v>1</v>
@@ -3456,10 +3456,10 @@
         <v>1</v>
       </c>
       <c r="H72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -3470,38 +3470,38 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Carlos Cañizares Estévez</t>
+          <t>Pawel Borkar</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>c.canizaresestevez@hotmail.com</t>
+          <t>36134699+PawelBorkar@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>PLAINCONCEPTS\ccanizares</t>
+          <t>Pawel Borkar</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>ccanizares@plainconcepts.com</t>
+          <t>36134699+pawelbr@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F73" t="b">
         <v>0</v>
       </c>
       <c r="G73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -3512,35 +3512,35 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Carlos Cañizares Estévez</t>
+          <t>Pawel Borkar</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>ccanizares@plainconcepts.com</t>
+          <t>36134699+PawelBorkar@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>PLAINCONCEPTS\ccanizares</t>
+          <t>PawelBorkar</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>ccanizares@plainconcepts.com</t>
+          <t>paawel@pm.me</t>
         </is>
       </c>
       <c r="E74" t="n">
         <v>0</v>
       </c>
       <c r="F74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I74" t="b">
         <v>0</v>
@@ -3554,38 +3554,38 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Unai</t>
+          <t>Pawel Borkar</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>unai@plainconcepts.com</t>
+          <t>36134699+pawelborkar@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>unaizorrilla</t>
+          <t>Pawel Borkar</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>unai@plainconcepts.com</t>
+          <t>36134699+pawelbr@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F75" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G75" t="b">
         <v>1</v>
       </c>
       <c r="H75" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I75" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -3596,35 +3596,35 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>unai</t>
+          <t>Pawel Borkar</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>unai@plainconcepts.com</t>
+          <t>36134699+pawelborkar@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>unaizorrilla</t>
+          <t>PawelBorkar</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>unai@plainconcepts.com</t>
+          <t>paawel@pm.me</t>
         </is>
       </c>
       <c r="E76" t="n">
         <v>0</v>
       </c>
       <c r="F76" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G76" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I76" t="b">
         <v>0</v>
@@ -3638,35 +3638,35 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>DESKTOP-V1VLQ15\dsanz</t>
+          <t>Pawel Borkar</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>dsanz@plainconcepts.com</t>
+          <t>36134699+pawelbr@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>David Sanz</t>
+          <t>PawelBorkar</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>dsanz@plainconcepts.com</t>
+          <t>paawel@pm.me</t>
         </is>
       </c>
       <c r="E77" t="n">
         <v>0</v>
       </c>
       <c r="F77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H77" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I77" t="b">
         <v>0</v>
@@ -3680,35 +3680,35 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Eric Torre</t>
+          <t>Pedro</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>etorreg@gmail.com</t>
+          <t>pcambra@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>ericuss</t>
+          <t>Pedro Cambra</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>etorre@gmail.com</t>
+          <t>pedro.cambra@gmail.com</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F78" t="b">
         <v>0</v>
       </c>
       <c r="G78" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I78" t="b">
         <v>0</v>
@@ -3722,35 +3722,35 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Eric Torre</t>
+          <t>Pt. Prashant tripathi</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>etorreg@gmail.com</t>
+          <t>26687933+PtPrashantTripathi@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>ericuss</t>
+          <t>ptprashanttripathi</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>etorreg@gmail.com</t>
+          <t>ptprashanttripathi@outlook.com</t>
         </is>
       </c>
       <c r="E79" t="n">
         <v>0</v>
       </c>
       <c r="F79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H79" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I79" t="b">
         <v>0</v>
@@ -3764,38 +3764,38 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Sychev Igor</t>
+          <t>SHARAD RAJ</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>igorsych@microsoft.com</t>
+          <t>36638057+sharadcodes@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>igorsych</t>
+          <t>Sharad Raj</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>igorsych@microsoft.com</t>
+          <t>dev_sharad@outlook.com</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F80" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G80" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H80" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I80" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -3806,26 +3806,26 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>eiximenis</t>
+          <t>Sent</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>etomas@gmail.com</t>
+          <t>66543853+sent@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>etomas</t>
+          <t>sent</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>etomas@gmail.com</t>
+          <t>66543853+sent@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F81" t="b">
         <v>1</v>
@@ -3834,10 +3834,10 @@
         <v>1</v>
       </c>
       <c r="H81" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I81" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -3848,32 +3848,32 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>epique@plainconcepts.com</t>
+          <t>Shatha Makhlouf</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>epique@plainconcepts.com</t>
+          <t>shada_m2006@yahoo.com</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>erikpique</t>
+          <t>biomedengsam</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>erik.pique@gmail.com</t>
+          <t>shada_m2006@yahoo.com</t>
         </is>
       </c>
       <c r="E82" t="n">
         <v>0</v>
       </c>
       <c r="F82" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G82" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82" t="b">
         <v>0</v>
@@ -3890,38 +3890,38 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Erik Pique</t>
+          <t>ShevAbam</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>epique@plainconcepts.com</t>
+          <t>shevabam@gmail.com</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>epique@plainconcepts.com</t>
+          <t>shevabam</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>epique@plainconcepts.com</t>
+          <t>shevabam@users.noreply.github.com</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F83" t="b">
         <v>1</v>
       </c>
       <c r="G83" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -3932,26 +3932,26 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Unai</t>
+          <t>Shivang Kaul</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>unai@plainconcepts.com</t>
+          <t>shangkaul@gmail.com</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Unai Zorrilla Castro</t>
+          <t>shangkaul</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>unai@plainconcepts.com</t>
+          <t>shangkaul@gmail.com</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>0.3333333333333333</v>
+        <v>0</v>
       </c>
       <c r="F84" t="b">
         <v>1</v>
@@ -3974,38 +3974,38 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Unai Zorrilla Castro</t>
+          <t>Shubham Jain</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>unai@plainconcepts.com</t>
+          <t>hi@shubhamjain.co</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>unai</t>
+          <t>Shubham Jain</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>unai@plainconcepts.com</t>
+          <t>shubham.jain.1@gmail.com</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="F85" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G85" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H85" t="b">
         <v>0</v>
       </c>
       <c r="I85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -4016,26 +4016,26 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Eduard Tomas</t>
+          <t>Travis</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>etomas@gmail.com</t>
+          <t>builds@travis-ci.org</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>eiximenis</t>
+          <t>Travis CI</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>etomas@gmail.com</t>
+          <t>builds@travis-ci.org</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F86" t="b">
         <v>1</v>
@@ -4058,38 +4058,38 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Eduard Tomàs</t>
+          <t>Travis CI</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>etomas@gmail.com</t>
+          <t>build@travis.org</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>eiximenis</t>
+          <t>Travis CI</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>etomas@gmail.com</t>
+          <t>builds@travis-ci.org</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H87" t="b">
         <v>0</v>
       </c>
       <c r="I87" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -4100,38 +4100,38 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Wenjie Yu（MSFT）</t>
+          <t>Vaibhav Mehta</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>81678720+zedy-wj@users.noreply.github.com</t>
+          <t>i-break-codes@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>zedy</t>
+          <t>Vaibhav Mehta</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>81678720+zedy-wj@users.noreply.github.com</t>
+          <t>vaibhav@browserstack.com</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F88" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G88" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H88" t="b">
         <v>1</v>
       </c>
       <c r="I88" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -4142,26 +4142,26 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>Visual Crossing Corporation</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>etorre@plainconcepts.com</t>
+          <t>52202145+visualcrossing@users.noreply.github.com</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Eric Torre</t>
+          <t>Visual Crossing Corporation</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>etorreg@gmail.com</t>
+          <t>info@visualcrossing.com</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F89" t="b">
         <v>0</v>
@@ -4170,10 +4170,10 @@
         <v>0</v>
       </c>
       <c r="H89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -4184,22 +4184,22 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>VojtaN</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>etorre@plainconcepts.com</t>
+          <t>vn@abalin.net</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>ericuss</t>
+          <t>nekvapil</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>etorre@gmail.com</t>
+          <t>vn@abalin.net</t>
         </is>
       </c>
       <c r="E90" t="n">
@@ -4209,7 +4209,7 @@
         <v>1</v>
       </c>
       <c r="G90" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H90" t="b">
         <v>0</v>
@@ -4226,32 +4226,32 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>VojtaN</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>etorre@plainconcepts.com</t>
+          <t>vn@abalin.net</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>ericuss</t>
+          <t>vne</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>etorreg@gmail.com</t>
+          <t>vn@abalin.net</t>
         </is>
       </c>
       <c r="E91" t="n">
         <v>0</v>
       </c>
       <c r="F91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H91" t="b">
         <v>0</v>
@@ -4260,6 +4260,510 @@
         <v>0</v>
       </c>
       <c r="J91" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Wes Bos</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>wesbos@gmail.com</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>wesbos</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>wesbos@gmail.com</t>
+        </is>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
+      <c r="F92" t="b">
+        <v>1</v>
+      </c>
+      <c r="G92" t="b">
+        <v>1</v>
+      </c>
+      <c r="H92" t="b">
+        <v>0</v>
+      </c>
+      <c r="I92" t="b">
+        <v>0</v>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>William Aboucaya</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>william.aboucaya@gmail.com</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>WilliamAboucaya</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>william.aboucaya@gmail.com</t>
+        </is>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+      <c r="F93" t="b">
+        <v>1</v>
+      </c>
+      <c r="G93" t="b">
+        <v>1</v>
+      </c>
+      <c r="H93" t="b">
+        <v>0</v>
+      </c>
+      <c r="I93" t="b">
+        <v>0</v>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Yann Bertrand</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>5855339+yannbertrand@users.noreply.github.com</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Yann Bertrand</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>github@yann-bertrand.fr</t>
+        </is>
+      </c>
+      <c r="E94" t="n">
+        <v>1</v>
+      </c>
+      <c r="F94" t="b">
+        <v>0</v>
+      </c>
+      <c r="G94" t="b">
+        <v>0</v>
+      </c>
+      <c r="H94" t="b">
+        <v>1</v>
+      </c>
+      <c r="I94" t="b">
+        <v>1</v>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Yann Bertrand</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>5855339+yannbertrand@users.noreply.github.com</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Yann Bertrand</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>yann@bertrand.com</t>
+        </is>
+      </c>
+      <c r="E95" t="n">
+        <v>1</v>
+      </c>
+      <c r="F95" t="b">
+        <v>0</v>
+      </c>
+      <c r="G95" t="b">
+        <v>0</v>
+      </c>
+      <c r="H95" t="b">
+        <v>1</v>
+      </c>
+      <c r="I95" t="b">
+        <v>1</v>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Yann Bertrand</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>github@yann-bertrand.fr</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Yann Bertrand</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>yann@bertrand.com</t>
+        </is>
+      </c>
+      <c r="E96" t="n">
+        <v>1</v>
+      </c>
+      <c r="F96" t="b">
+        <v>0</v>
+      </c>
+      <c r="G96" t="b">
+        <v>0</v>
+      </c>
+      <c r="H96" t="b">
+        <v>0</v>
+      </c>
+      <c r="I96" t="b">
+        <v>1</v>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>apilayer</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>support@apilayer.net</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>apilayer-admin</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>75280960+apilayer-admin@users.noreply.github.com</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F97" t="b">
+        <v>0</v>
+      </c>
+      <c r="G97" t="b">
+        <v>0</v>
+      </c>
+      <c r="H97" t="b">
+        <v>1</v>
+      </c>
+      <c r="I97" t="b">
+        <v>0</v>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>arian firoozfar</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>polarspetroll@gmail.com</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>polarspetroll</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>polarspetroll@gmail.com</t>
+        </is>
+      </c>
+      <c r="E98" t="n">
+        <v>0</v>
+      </c>
+      <c r="F98" t="b">
+        <v>1</v>
+      </c>
+      <c r="G98" t="b">
+        <v>1</v>
+      </c>
+      <c r="H98" t="b">
+        <v>0</v>
+      </c>
+      <c r="I98" t="b">
+        <v>0</v>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>bittricky</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>39785177+bittricky@users.noreply.github.com</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>bittricky</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>me@mitulpa.tel</t>
+        </is>
+      </c>
+      <c r="E99" t="n">
+        <v>1</v>
+      </c>
+      <c r="F99" t="b">
+        <v>0</v>
+      </c>
+      <c r="G99" t="b">
+        <v>0</v>
+      </c>
+      <c r="H99" t="b">
+        <v>1</v>
+      </c>
+      <c r="I99" t="b">
+        <v>1</v>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>ismael</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>bychis6@gmail.com</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>ismael</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>tomas.verdugo@ug.uchile.cl</t>
+        </is>
+      </c>
+      <c r="E100" t="n">
+        <v>1</v>
+      </c>
+      <c r="F100" t="b">
+        <v>0</v>
+      </c>
+      <c r="G100" t="b">
+        <v>0</v>
+      </c>
+      <c r="H100" t="b">
+        <v>0</v>
+      </c>
+      <c r="I100" t="b">
+        <v>1</v>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>nekvapil</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>vn@abalin.net</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>vne</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>vn@abalin.net</t>
+        </is>
+      </c>
+      <c r="E101" t="n">
+        <v>0</v>
+      </c>
+      <c r="F101" t="b">
+        <v>1</v>
+      </c>
+      <c r="G101" t="b">
+        <v>1</v>
+      </c>
+      <c r="H101" t="b">
+        <v>0</v>
+      </c>
+      <c r="I101" t="b">
+        <v>0</v>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>sha016</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>92833633+sha016@users.noreply.github.com</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>sha016</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>sha0160@protonmail.com</t>
+        </is>
+      </c>
+      <c r="E102" t="n">
+        <v>1</v>
+      </c>
+      <c r="F102" t="b">
+        <v>0</v>
+      </c>
+      <c r="G102" t="b">
+        <v>0</v>
+      </c>
+      <c r="H102" t="b">
+        <v>1</v>
+      </c>
+      <c r="I102" t="b">
+        <v>1</v>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>zag2me</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>doowles2@hotmail.com</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>zag2me</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>zag@kodi.tv</t>
+        </is>
+      </c>
+      <c r="E103" t="n">
+        <v>1</v>
+      </c>
+      <c r="F103" t="b">
+        <v>0</v>
+      </c>
+      <c r="G103" t="b">
+        <v>0</v>
+      </c>
+      <c r="H103" t="b">
+        <v>0</v>
+      </c>
+      <c r="I103" t="b">
+        <v>1</v>
+      </c>
+      <c r="J103" t="inlineStr">
         <is>
           <t>FP</t>
         </is>

</xml_diff>